<commit_message>
chng to dist table
</commit_message>
<xml_diff>
--- a/data/PriorModel/Dist_table.xlsx
+++ b/data/PriorModel/Dist_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Samsung_T5/ProjectsLocal/SWIlarge/data/PriorModel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A561B8-8EAC-EF43-9326-E1544AC89435}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF47382F-D3AB-DD42-BDF8-065BD3040E84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="4700" windowWidth="36100" windowHeight="19720" xr2:uid="{74934045-B491-2F42-B546-A1424287AB4A}"/>
+    <workbookView xWindow="15120" yWindow="2380" windowWidth="23500" windowHeight="18460" xr2:uid="{74934045-B491-2F42-B546-A1424287AB4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
   <si>
     <t>Group</t>
   </si>
@@ -212,9 +212,6 @@
     <t>U~[.25,.55]</t>
   </si>
   <si>
-    <t>Geophysics</t>
-  </si>
-  <si>
     <t>Layer 1</t>
   </si>
   <si>
@@ -224,13 +221,31 @@
     <t>LU~[100,1000]</t>
   </si>
   <si>
-    <t>U~[.3,3]</t>
-  </si>
-  <si>
-    <t>U~[1e-2,1e-1]</t>
-  </si>
-  <si>
     <t>U~[0.25,1.0]</t>
+  </si>
+  <si>
+    <t>DSA_yn</t>
+  </si>
+  <si>
+    <t>P=[0.1,0.9]</t>
+  </si>
+  <si>
+    <t>U~[.6,4]</t>
+  </si>
+  <si>
+    <t>BC_change</t>
+  </si>
+  <si>
+    <t>U~[-5,5]</t>
+  </si>
+  <si>
+    <t>U~[1e-2,1e-0]</t>
+  </si>
+  <si>
+    <t>U~[1e-2,1e0]</t>
+  </si>
+  <si>
+    <t>Rock physics</t>
   </si>
 </sst>
 </file>
@@ -267,18 +282,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -293,7 +302,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -302,26 +311,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <top style="thin">
+        <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -329,9 +329,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -342,9 +340,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -353,9 +349,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -363,12 +357,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -378,11 +376,84 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -390,60 +461,70 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -760,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEE23B2-0CA5-5A45-905F-B1020E467ACD}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="223" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -775,344 +856,360 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="10"/>
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="8"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="3" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D7" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="3" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D8" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="3" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D9" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="3" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="3" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="16" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D12" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="3" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D13" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13">
-        <f>E13*0.3048</f>
-        <v>0.60960000000000003</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14">
-        <v>10</v>
-      </c>
-      <c r="F14">
-        <f>E14*0.3048</f>
-        <v>3.048</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="7" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="14"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D18" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="7" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="14"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D19" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="7" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="14"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D20" s="13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="7" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="14"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D21" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="14"/>
+      <c r="B22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D22" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="7" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="14"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="D23" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="D24" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="7" t="s">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="7" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="16"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D26" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="3" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D27" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="3" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="17"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D28" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="3" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="17"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D29" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="3" t="s">
+    <row r="30" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D30" s="20" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A16"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A17:A23"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A14"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>